<commit_message>
DDM and Bendigo Excel
</commit_message>
<xml_diff>
--- a/Assignment_Body/BENDIGO.xlsx
+++ b/Assignment_Body/BENDIGO.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d43dd5ddc1e2bd78/Desktop/BAFE/2025 SEM1/FINM3422/Equity Research Assignment/Group_46_FM_equity_research-/Assignment_Body/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{E0F5F173-72F3-480B-9CA3-4C76A4C705EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43764F64-D365-4D49-AE12-8ABAF9070BB9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC1313DA-7C97-4C41-A132-F938AF626DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{C40C285E-7926-4BFA-A8EA-1C74888DBDA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dividend Discount Model" sheetId="1" r:id="rId1"/>
+    <sheet name="Cost of Equity" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>FY2025</t>
   </si>
@@ -168,6 +169,24 @@
   </si>
   <si>
     <t>Discount/(Premium)</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Risk Free Rate</t>
+  </si>
+  <si>
+    <t>MRP</t>
+  </si>
+  <si>
+    <t>&lt;--- KPMG MRP</t>
+  </si>
+  <si>
+    <t>&lt;--- 28/0425 10yr Australian Gov Bond</t>
+  </si>
+  <si>
+    <t>&lt;--- Bloomberg</t>
   </si>
 </sst>
 </file>
@@ -180,9 +199,9 @@
     <numFmt numFmtId="165" formatCode="#,##0.00;\(#,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="#,##0.00_);\(#,##0.00\);@_)"/>
     <numFmt numFmtId="167" formatCode="0.000000000"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000000000_);\(#,##0.000000000\);@_)"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00%_);\ \(#,##0.00%\);\ &quot;-&quot;;\ @"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +319,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -378,7 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -422,6 +456,7 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -443,8 +478,10 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -454,8 +491,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FF8C0A42"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FFFF5357"/>
       <color rgb="FFAC0440"/>
       <color rgb="FFFF3338"/>
@@ -792,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314E70D6-0A07-40D1-BF88-F5CE50014335}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="74" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="82" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -942,7 +979,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="43">
+      <c r="J9" s="44">
         <v>45772</v>
       </c>
       <c r="K9" s="6"/>
@@ -961,14 +998,14 @@
       <c r="D10" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="44">
+      <c r="J10" s="45">
         <v>10.88</v>
       </c>
       <c r="K10" s="6"/>
@@ -987,18 +1024,18 @@
       <c r="D11" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="37" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="41">
+      <c r="J11" s="42">
         <v>566.54</v>
       </c>
       <c r="K11" s="6"/>
-      <c r="L11" s="37"/>
+      <c r="L11" s="38"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
@@ -1013,15 +1050,16 @@
       <c r="D12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="37" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="45">
-        <v>7.9000000000000001E-2</v>
+      <c r="J12" s="46">
+        <f>'Cost of Equity'!E12</f>
+        <v>8.6900000000000005E-2</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1039,15 +1077,15 @@
       <c r="D13" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="37" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="45">
-        <v>2.1000000000000001E-2</v>
+      <c r="J13" s="46">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1075,20 +1113,20 @@
     </row>
     <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15"/>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B16" s="6"/>
@@ -1131,7 +1169,7 @@
       </c>
       <c r="E18" s="34">
         <f>J49</f>
-        <v>11.561081140384864</v>
+        <v>10.729244797114228</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -1148,9 +1186,9 @@
       <c r="D19" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E19" s="53">
         <f>E18/E17-1</f>
-        <v>6.2599369520667691E-2</v>
+        <v>-1.3856176735824621E-2</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -1177,26 +1215,26 @@
     </row>
     <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21"/>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B22" s="6"/>
@@ -1218,7 +1256,7 @@
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
     </row>
-    <row r="23" spans="1:19" s="53" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8" t="s">
@@ -1275,19 +1313,19 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="14"/>
-      <c r="K25" s="42">
+      <c r="K25" s="43">
         <f>$J$11</f>
         <v>566.54</v>
       </c>
-      <c r="L25" s="42">
+      <c r="L25" s="43">
         <f t="shared" ref="L25:M25" si="0">$J$11</f>
         <v>566.54</v>
       </c>
-      <c r="M25" s="42">
+      <c r="M25" s="43">
         <f t="shared" si="0"/>
         <v>566.54</v>
       </c>
-      <c r="N25" s="46">
+      <c r="N25" s="47">
         <f>M25</f>
         <v>566.54</v>
       </c>
@@ -1323,28 +1361,28 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="17"/>
-      <c r="K26" s="41">
+      <c r="K26" s="42">
         <v>488.1</v>
       </c>
-      <c r="L26" s="41">
+      <c r="L26" s="42">
         <v>497</v>
       </c>
-      <c r="M26" s="40">
+      <c r="M26" s="41">
         <v>545</v>
       </c>
-      <c r="N26" s="41">
+      <c r="N26" s="42">
         <v>455.86</v>
       </c>
-      <c r="O26" s="41">
+      <c r="O26" s="42">
         <v>491.76</v>
       </c>
-      <c r="P26" s="41">
+      <c r="P26" s="42">
         <v>500.55</v>
       </c>
-      <c r="Q26" s="41">
+      <c r="Q26" s="42">
         <v>515.5</v>
       </c>
-      <c r="R26" s="41">
+      <c r="R26" s="42">
         <v>611</v>
       </c>
       <c r="S26" s="7"/>
@@ -1479,35 +1517,35 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="20"/>
-      <c r="K30" s="49">
+      <c r="K30" s="50">
         <f>K27/K26</f>
         <v>0.61517353001434127</v>
       </c>
-      <c r="L30" s="49">
+      <c r="L30" s="50">
         <f t="shared" ref="L30:M30" si="4">L27/L26</f>
         <v>0.69535090543259548</v>
       </c>
-      <c r="M30" s="50">
+      <c r="M30" s="51">
         <f t="shared" si="4"/>
         <v>0.65489944954128432</v>
       </c>
-      <c r="N30" s="49">
+      <c r="N30" s="50">
         <f>AVERAGE($K$30:$M$30)</f>
         <v>0.65514129499607365</v>
       </c>
-      <c r="O30" s="49">
+      <c r="O30" s="50">
         <f t="shared" ref="O30:R30" si="5">AVERAGE($K$30:$M$30)</f>
         <v>0.65514129499607365</v>
       </c>
-      <c r="P30" s="49">
+      <c r="P30" s="50">
         <f t="shared" si="5"/>
         <v>0.65514129499607365</v>
       </c>
-      <c r="Q30" s="49">
+      <c r="Q30" s="50">
         <f t="shared" si="5"/>
         <v>0.65514129499607365</v>
       </c>
-      <c r="R30" s="49">
+      <c r="R30" s="50">
         <f t="shared" si="5"/>
         <v>0.65514129499607365</v>
       </c>
@@ -1527,13 +1565,13 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="20"/>
-      <c r="K31" s="47">
+      <c r="K31" s="48">
         <v>0.53</v>
       </c>
-      <c r="L31" s="47">
+      <c r="L31" s="48">
         <v>0.61</v>
       </c>
-      <c r="M31" s="48">
+      <c r="M31" s="49">
         <v>0.63</v>
       </c>
       <c r="N31" s="22">
@@ -1673,25 +1711,25 @@
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
       <c r="M35" s="29"/>
-      <c r="N35" s="54">
+      <c r="N35" s="30">
         <f>N31/(1+$J$12)^N34</f>
-        <v>0.51995395001129951</v>
-      </c>
-      <c r="O35" s="54">
-        <f t="shared" ref="O35:R35" si="9">O31/(1+$J$12)^O34</f>
-        <v>0.51983456227040392</v>
-      </c>
-      <c r="P35" s="54">
-        <f t="shared" si="9"/>
-        <v>0.49038589720305303</v>
-      </c>
-      <c r="Q35" s="54">
-        <f t="shared" si="9"/>
-        <v>0.46795841520611259</v>
-      </c>
-      <c r="R35" s="54">
-        <f t="shared" si="9"/>
-        <v>0.51404170742377364</v>
+        <v>0.51926854044587989</v>
+      </c>
+      <c r="O35" s="30">
+        <f>O31/(1+$J$12)^O34</f>
+        <v>0.51537593668224113</v>
+      </c>
+      <c r="P35" s="30">
+        <f>P31/(1+$J$12)^P34</f>
+        <v>0.48264611414623587</v>
+      </c>
+      <c r="Q35" s="30">
+        <f>Q31/(1+$J$12)^Q34</f>
+        <v>0.45721585230009781</v>
+      </c>
+      <c r="R35" s="30">
+        <f>R31/(1+$J$12)^R34</f>
+        <v>0.49859076647723988</v>
       </c>
       <c r="S35" s="27"/>
     </row>
@@ -1730,7 +1768,7 @@
       <c r="I37" s="6"/>
       <c r="J37" s="32">
         <f>SUM(N35:R35)</f>
-        <v>2.5121745321146425</v>
+        <v>2.4730972100516948</v>
       </c>
       <c r="K37" s="18"/>
       <c r="L37" s="18"/>
@@ -1782,7 +1820,7 @@
       <c r="R39" s="6"/>
       <c r="S39" s="6"/>
     </row>
-    <row r="40" spans="1:19" s="53" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40"/>
       <c r="B40" s="6"/>
       <c r="C40" s="8" t="s">
@@ -1865,9 +1903,9 @@
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
-      <c r="J43" s="55">
+      <c r="J43" s="35">
         <f>J13</f>
-        <v>2.1000000000000001E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
@@ -1894,7 +1932,7 @@
       <c r="I44" s="6"/>
       <c r="J44" s="34">
         <f>J42*(1+J43)</f>
-        <v>0.72139204504306065</v>
+        <v>0.72421826265341549</v>
       </c>
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
@@ -1921,7 +1959,7 @@
       <c r="I45" s="6"/>
       <c r="J45" s="34">
         <f>J44/(J12-J43)</f>
-        <v>12.437793880052771</v>
+        <v>11.699810382123028</v>
       </c>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
@@ -1975,7 +2013,7 @@
       <c r="I47" s="27"/>
       <c r="J47" s="30">
         <f>J45/(1+J12)^J46</f>
-        <v>9.0489066082702223</v>
+        <v>8.256147587062534</v>
       </c>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -2002,7 +2040,7 @@
       <c r="I48" s="6"/>
       <c r="J48" s="34">
         <f>$J$37</f>
-        <v>2.5121745321146425</v>
+        <v>2.4730972100516948</v>
       </c>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
@@ -2027,9 +2065,9 @@
       <c r="G49" s="27"/>
       <c r="H49" s="27"/>
       <c r="I49" s="27"/>
-      <c r="J49" s="35">
+      <c r="J49" s="36">
         <f>SUM(J47:J48)</f>
-        <v>11.561081140384864</v>
+        <v>10.729244797114228</v>
       </c>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
@@ -2043,26 +2081,126 @@
     </row>
     <row r="51" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51"/>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="39"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="39"/>
-      <c r="K51" s="39"/>
-      <c r="L51" s="39"/>
-      <c r="M51" s="39"/>
-      <c r="N51" s="39"/>
-      <c r="O51" s="39"/>
-      <c r="P51" s="39"/>
-      <c r="Q51" s="39"/>
-      <c r="R51" s="39"/>
-      <c r="S51" s="39"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="40"/>
+      <c r="J51" s="40"/>
+      <c r="K51" s="40"/>
+      <c r="L51" s="40"/>
+      <c r="M51" s="40"/>
+      <c r="N51" s="40"/>
+      <c r="O51" s="40"/>
+      <c r="P51" s="40"/>
+      <c r="Q51" s="40"/>
+      <c r="R51" s="40"/>
+      <c r="S51" s="40"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD4471B-DA51-46B0-897F-B3A7744DA7FF}">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="1.73046875" customWidth="1"/>
+    <col min="3" max="3" width="28.59765625" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="A2"/>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A3"/>
+      <c r="B3" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="57">
+        <v>0.91</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="58">
+        <v>4.1399999999999999E-2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="58">
+        <v>0.05</v>
+      </c>
+      <c r="G11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C12" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56">
+        <f>E10+E11*E9</f>
+        <v>8.6900000000000005E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>